<commit_message>
Lógoca de funcionamento ok
</commit_message>
<xml_diff>
--- a/transacoes.xlsx
+++ b/transacoes.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mesada</t>
+          <t>Salário</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>4892</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,11 +501,11 @@
         <v>9</v>
       </c>
       <c r="H2" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>16:29:16</t>
+          <t>11:07:28</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bombom</t>
+          <t xml:space="preserve"> Uber</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lazer</t>
+          <t>Transporte</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 55</t>
+          <t xml:space="preserve"> 5.45</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -542,11 +542,11 @@
         <v>9</v>
       </c>
       <c r="H3" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>16:30:01</t>
+          <t>11:07:44</t>
         </is>
       </c>
     </row>
@@ -558,17 +558,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gdfg</t>
+          <t xml:space="preserve"> pão</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Moradia</t>
+          <t>Alimento</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 897</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -576,92 +576,92 @@
           <t>Cartão</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>09</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F4" t="n">
+        <v>2024</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>21</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>16:31:00</t>
+          <t>11:08:18</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Entrada</t>
+          <t>Saída</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gfdgf</t>
+          <t xml:space="preserve"> Festa</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Lazer</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>897</t>
+          <t xml:space="preserve"> 256.59</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dinheiro</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2024</v>
-      </c>
-      <c r="G5" t="n">
-        <v>9</v>
-      </c>
-      <c r="H5" t="n">
-        <v>18</v>
+          <t>Fiado</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>16:32:45</t>
+          <t>11:14:54</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Saída</t>
+          <t>Entrada</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>sida</t>
+          <t>dfr</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Alimento</t>
+          <t>Outros</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>445</t>
+          <t>59</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dinheiro</t>
+          <t>Fiado</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -671,38 +671,38 @@
         <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>16:43:32</t>
+          <t>12:06:28</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Entrada</t>
+          <t>Saída</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 89</t>
+          <t>cerveja</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Lazer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 89</t>
+          <t>89</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dinheiro</t>
+          <t>Pix</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -712,11 +712,11 @@
         <v>9</v>
       </c>
       <c r="H7" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>16:43:56</t>
+          <t>13:54:19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Primeirs analise de dados
</commit_message>
<xml_diff>
--- a/transacoes.xlsx
+++ b/transacoes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="200">
   <si>
     <t>Tipo</t>
   </si>
@@ -602,6 +602,18 @@
   </si>
   <si>
     <t>13.18</t>
+  </si>
+  <si>
+    <t>Cartão</t>
+  </si>
+  <si>
+    <t>Fiado</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>Dinheiro</t>
   </si>
 </sst>
 </file>
@@ -637,8 +649,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1059,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F4">
         <v>2024</v>
@@ -1098,7 +1111,7 @@
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F6">
         <v>2024</v>
@@ -1150,7 +1163,7 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F8">
         <v>2024</v>
@@ -1202,7 +1215,7 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F10">
         <v>2024</v>
@@ -1254,7 +1267,7 @@
         <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F12">
         <v>2024</v>
@@ -1332,7 +1345,7 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F15">
         <v>2024</v>
@@ -1358,7 +1371,7 @@
         <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F16">
         <v>2024</v>
@@ -1436,7 +1449,7 @@
         <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F19">
         <v>2024</v>
@@ -1514,7 +1527,7 @@
         <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F22">
         <v>2024</v>
@@ -1618,7 +1631,7 @@
         <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F26">
         <v>2024</v>
@@ -1696,7 +1709,7 @@
         <v>58</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F29">
         <v>2024</v>
@@ -1774,7 +1787,7 @@
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F32">
         <v>2024</v>
@@ -1878,7 +1891,7 @@
         <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F36">
         <v>2024</v>
@@ -1956,7 +1969,7 @@
         <v>74</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F39">
         <v>2024</v>
@@ -2034,7 +2047,7 @@
         <v>76</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F42">
         <v>2024</v>
@@ -2120,7 +2133,7 @@
       <c r="G45">
         <v>9</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="1">
         <v>9</v>
       </c>
     </row>
@@ -2138,7 +2151,7 @@
         <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F46">
         <v>2024</v>
@@ -2190,7 +2203,7 @@
         <v>83</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F48">
         <v>2024</v>
@@ -2294,7 +2307,7 @@
         <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F52">
         <v>2024</v>
@@ -2372,7 +2385,7 @@
         <v>88</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F55">
         <v>2024</v>
@@ -2450,7 +2463,7 @@
         <v>93</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F58">
         <v>2024</v>
@@ -2528,7 +2541,7 @@
         <v>38</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F61">
         <v>2024</v>
@@ -2606,7 +2619,7 @@
         <v>96</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F64">
         <v>2024</v>
@@ -2684,7 +2697,7 @@
         <v>97</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F67">
         <v>2024</v>
@@ -2736,7 +2749,7 @@
         <v>99</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F69">
         <v>2024</v>
@@ -2800,7 +2813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -2814,7 +2827,7 @@
         <v>90</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F72">
         <v>2024</v>
@@ -2892,7 +2905,7 @@
         <v>103</v>
       </c>
       <c r="E75" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F75">
         <v>2024</v>
@@ -2944,7 +2957,7 @@
         <v>105</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F77">
         <v>2024</v>
@@ -2956,7 +2969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -2996,7 +3009,7 @@
         <v>106</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F79">
         <v>2024</v>
@@ -3048,7 +3061,7 @@
         <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F81">
         <v>2024</v>
@@ -3126,7 +3139,7 @@
         <v>109</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F84">
         <v>2024</v>
@@ -3190,7 +3203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -3204,7 +3217,7 @@
         <v>35</v>
       </c>
       <c r="E87" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F87">
         <v>2024</v>
@@ -3256,7 +3269,7 @@
         <v>33</v>
       </c>
       <c r="E89" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F89">
         <v>2024</v>
@@ -3308,7 +3321,7 @@
         <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F91">
         <v>2024</v>
@@ -3386,7 +3399,7 @@
         <v>62</v>
       </c>
       <c r="E94" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F94">
         <v>2024</v>
@@ -3438,7 +3451,7 @@
         <v>115</v>
       </c>
       <c r="E96" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F96">
         <v>2024</v>
@@ -3490,7 +3503,7 @@
         <v>117</v>
       </c>
       <c r="E98" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F98">
         <v>2024</v>
@@ -3502,7 +3515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -3568,7 +3581,7 @@
         <v>17</v>
       </c>
       <c r="E101" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F101">
         <v>2024</v>
@@ -3620,7 +3633,7 @@
         <v>120</v>
       </c>
       <c r="E103" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F103">
         <v>2024</v>
@@ -3698,7 +3711,7 @@
         <v>122</v>
       </c>
       <c r="E106" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F106">
         <v>2024</v>
@@ -3750,7 +3763,7 @@
         <v>123</v>
       </c>
       <c r="E108" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F108">
         <v>2024</v>
@@ -3802,7 +3815,7 @@
         <v>123</v>
       </c>
       <c r="E110" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F110">
         <v>2024</v>
@@ -3854,7 +3867,7 @@
         <v>126</v>
       </c>
       <c r="E112" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F112">
         <v>2024</v>
@@ -3906,7 +3919,7 @@
         <v>22</v>
       </c>
       <c r="E114" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F114">
         <v>2024</v>
@@ -3944,7 +3957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -3958,7 +3971,7 @@
         <v>48</v>
       </c>
       <c r="E116" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F116">
         <v>2024</v>
@@ -4010,7 +4023,7 @@
         <v>92</v>
       </c>
       <c r="E118" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F118">
         <v>2024</v>
@@ -4036,7 +4049,7 @@
         <v>73</v>
       </c>
       <c r="E119" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F119">
         <v>2024</v>
@@ -4114,7 +4127,7 @@
         <v>130</v>
       </c>
       <c r="E122" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F122">
         <v>2024</v>
@@ -4166,7 +4179,7 @@
         <v>38</v>
       </c>
       <c r="E124" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F124">
         <v>2024</v>
@@ -4218,7 +4231,7 @@
         <v>132</v>
       </c>
       <c r="E126" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F126">
         <v>2024</v>
@@ -4244,7 +4257,7 @@
         <v>133</v>
       </c>
       <c r="E127" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F127">
         <v>2024</v>
@@ -4256,7 +4269,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -4348,7 +4361,7 @@
         <v>62</v>
       </c>
       <c r="E131" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F131">
         <v>2024</v>
@@ -4400,7 +4413,7 @@
         <v>137</v>
       </c>
       <c r="E133" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F133">
         <v>2024</v>
@@ -4438,7 +4451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -4504,7 +4517,7 @@
         <v>139</v>
       </c>
       <c r="E137" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F137">
         <v>2024</v>
@@ -4568,7 +4581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -4582,7 +4595,7 @@
         <v>73</v>
       </c>
       <c r="E140" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F140">
         <v>2024</v>
@@ -4646,7 +4659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -4660,7 +4673,7 @@
         <v>143</v>
       </c>
       <c r="E143" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F143">
         <v>2024</v>
@@ -4712,7 +4725,7 @@
         <v>146</v>
       </c>
       <c r="E145" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="F145">
         <v>2024</v>
@@ -4790,7 +4803,7 @@
         <v>148</v>
       </c>
       <c r="E148" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F148">
         <v>2024</v>
@@ -4842,7 +4855,7 @@
         <v>150</v>
       </c>
       <c r="E150" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F150">
         <v>2024</v>
@@ -4894,7 +4907,7 @@
         <v>152</v>
       </c>
       <c r="E152" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F152">
         <v>2024</v>
@@ -4946,7 +4959,7 @@
         <v>155</v>
       </c>
       <c r="E154" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F154">
         <v>2024</v>
@@ -5050,7 +5063,7 @@
         <v>158</v>
       </c>
       <c r="E158" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F158">
         <v>2024</v>
@@ -5128,7 +5141,7 @@
         <v>44</v>
       </c>
       <c r="E161" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F161">
         <v>2024</v>
@@ -5206,7 +5219,7 @@
         <v>38</v>
       </c>
       <c r="E164" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F164">
         <v>2024</v>
@@ -5258,7 +5271,7 @@
         <v>66</v>
       </c>
       <c r="E166" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F166">
         <v>2024</v>
@@ -5296,7 +5309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -5310,7 +5323,7 @@
         <v>33</v>
       </c>
       <c r="E168" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F168">
         <v>2024</v>
@@ -5374,7 +5387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -5414,7 +5427,7 @@
         <v>167</v>
       </c>
       <c r="E172" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="F172">
         <v>2024</v>
@@ -5452,7 +5465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>9</v>
       </c>
@@ -5466,7 +5479,7 @@
         <v>170</v>
       </c>
       <c r="E174" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F174">
         <v>2024</v>
@@ -5478,7 +5491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>9</v>
       </c>
@@ -5570,7 +5583,7 @@
         <v>174</v>
       </c>
       <c r="E178" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F178">
         <v>2024</v>
@@ -5582,7 +5595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>9</v>
       </c>
@@ -5648,7 +5661,7 @@
         <v>177</v>
       </c>
       <c r="E181" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="F181">
         <v>2024</v>
@@ -5686,7 +5699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>9</v>
       </c>
@@ -5700,7 +5713,7 @@
         <v>106</v>
       </c>
       <c r="E183" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F183">
         <v>2024</v>
@@ -5752,7 +5765,7 @@
         <v>33</v>
       </c>
       <c r="E185" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F185">
         <v>2024</v>
@@ -5764,7 +5777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -5804,7 +5817,7 @@
         <v>33</v>
       </c>
       <c r="E187" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F187">
         <v>2024</v>
@@ -5946,7 +5959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>9</v>
       </c>
@@ -5986,7 +5999,7 @@
         <v>90</v>
       </c>
       <c r="E194" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F194">
         <v>2024</v>
@@ -6024,7 +6037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -6284,7 +6297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>9</v>
       </c>
@@ -6324,7 +6337,7 @@
         <v>83</v>
       </c>
       <c r="E207" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="F207">
         <v>2024</v>

</xml_diff>